<commit_message>
Creation of Manifests and ManifestReference using Excel. New Table tpa_manifest. Manifest and ManifestReference have connection with TPA. Enums for TPA and TTT Status
</commit_message>
<xml_diff>
--- a/excelTemps/references.xlsx
+++ b/excelTemps/references.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UBU\_XDMS\excelTemps\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -63,12 +63,6 @@
     <t>PALLET PARAMETERS</t>
   </si>
   <si>
-    <t>Per Package</t>
-  </si>
-  <si>
-    <t>Per Handling Unit</t>
-  </si>
-  <si>
     <t>AGREEMENT</t>
   </si>
   <si>
@@ -88,6 +82,12 @@
   </si>
   <si>
     <t>DESIGNATION RU</t>
+  </si>
+  <si>
+    <t>PCS Per PU</t>
+  </si>
+  <si>
+    <t>PU per HU</t>
   </si>
 </sst>
 </file>
@@ -299,43 +299,43 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,119 +649,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="G1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="2" t="s">
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="2" t="s">
+      <c r="Q1" s="10"/>
+      <c r="R1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="4"/>
+      <c r="S1" s="10"/>
       <c r="T1" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="10" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="5" t="s">
+      <c r="R2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>15</v>
+      <c r="S2" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="T2" s="16"/>
-      <c r="U2" s="14"/>
+      <c r="U2" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:U2"/>
   <mergeCells count="15">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>